<commit_message>
Work on WB for Scene
Models Added and Adjusted
</commit_message>
<xml_diff>
--- a/Home Work Log.xlsx
+++ b/Home Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kand8\Documents\School 19-20\Modeling\2210Fall2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89B0F88-A537-416F-B3CE-D94E8863C653}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80D19ED-7335-4993-9D59-D9881BD8B00A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C211A382-238B-4D9E-A57D-3E5511C52C68}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date:</t>
   </si>
@@ -70,13 +70,19 @@
     </r>
   </si>
   <si>
-    <t>10:20AM-</t>
-  </si>
-  <si>
     <t>Week A:</t>
   </si>
   <si>
     <t>(Thursday) September 12, 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:20AM-11:11AM; </t>
+  </si>
+  <si>
+    <t>11:11AM-1:40PM;</t>
+  </si>
+  <si>
+    <t>1:44PM-3:36PM</t>
   </si>
 </sst>
 </file>
@@ -464,7 +470,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,15 +506,21 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>